<commit_message>
PET calculator now can use MACA data
</commit_message>
<xml_diff>
--- a/ClimateStatsforDCEW.xlsx
+++ b/ClimateStatsforDCEW.xlsx
@@ -64,13 +64,13 @@
     <t>BRW</t>
   </si>
   <si>
-    <t>Average temp stats</t>
+    <t>decrease precipitation 10% depth</t>
   </si>
   <si>
-    <t>increase precipitation 10% depth</t>
+    <t>Average temp and precip stats</t>
   </si>
   <si>
-    <t>decrease precipitation 10% depth</t>
+    <t>increase precipitation by 10% depth and temp with MACA R4.5 data</t>
   </si>
 </sst>
 </file>
@@ -597,11 +597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377264864"/>
-        <c:axId val="377274112"/>
+        <c:axId val="251005680"/>
+        <c:axId val="251005136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377274112"/>
+        <c:axId val="251005136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,12 +647,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377264864"/>
+        <c:crossAx val="251005680"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377264864"/>
+        <c:axId val="251005680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +680,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="377274112"/>
+        <c:crossAx val="251005136"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -946,11 +946,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377265408"/>
-        <c:axId val="377279008"/>
+        <c:axId val="251010032"/>
+        <c:axId val="251014928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377279008"/>
+        <c:axId val="251014928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,12 +996,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377265408"/>
+        <c:crossAx val="251010032"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377265408"/>
+        <c:axId val="251010032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,7 +1029,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="377279008"/>
+        <c:crossAx val="251014928"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1295,11 +1295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377275200"/>
-        <c:axId val="377270848"/>
+        <c:axId val="415260880"/>
+        <c:axId val="415266320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377270848"/>
+        <c:axId val="415266320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1345,12 +1345,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377275200"/>
+        <c:crossAx val="415260880"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377275200"/>
+        <c:axId val="415260880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,7 +1378,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="377270848"/>
+        <c:crossAx val="415266320"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1644,11 +1644,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377275744"/>
-        <c:axId val="377278464"/>
+        <c:axId val="415270128"/>
+        <c:axId val="415258704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377278464"/>
+        <c:axId val="415258704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1694,12 +1694,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377275744"/>
+        <c:crossAx val="415270128"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377275744"/>
+        <c:axId val="415270128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1727,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="377278464"/>
+        <c:crossAx val="415258704"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1993,11 +1993,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377269216"/>
-        <c:axId val="377267584"/>
+        <c:axId val="415260336"/>
+        <c:axId val="415258160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377267584"/>
+        <c:axId val="415258160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2043,12 +2043,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377269216"/>
+        <c:crossAx val="415260336"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377269216"/>
+        <c:axId val="415260336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2076,7 +2076,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="377267584"/>
+        <c:crossAx val="415258160"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2342,11 +2342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377272480"/>
-        <c:axId val="377271392"/>
+        <c:axId val="415264144"/>
+        <c:axId val="415267408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377271392"/>
+        <c:axId val="415267408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2392,12 +2392,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377272480"/>
+        <c:crossAx val="415264144"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377272480"/>
+        <c:axId val="415264144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,7 +2425,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="377271392"/>
+        <c:crossAx val="415267408"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3032,11 +3032,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="377397952"/>
-        <c:axId val="377396320"/>
+        <c:axId val="415265232"/>
+        <c:axId val="415263056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="377397952"/>
+        <c:axId val="415265232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,12 +3046,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="377396320"/>
+        <c:crossAx val="415263056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="377396320"/>
+        <c:axId val="415263056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.4"/>
@@ -3159,7 +3159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="377397952"/>
+        <c:crossAx val="415265232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4240,10 +4240,10 @@
   <dimension ref="A1:AL8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AA5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ17" sqref="AJ17"/>
+      <selection pane="bottomRight" activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4287,12 +4287,12 @@
   <sheetData>
     <row r="1" spans="1:38">
       <c r="C1" s="21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="O1" s="22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
@@ -4300,7 +4300,7 @@
       <c r="S1" s="22"/>
       <c r="T1" s="22"/>
       <c r="AA1" s="22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AB1" s="22"/>
       <c r="AC1" s="22"/>
@@ -4481,15 +4481,9 @@
       <c r="N4" s="14">
         <v>4.0599999999999996</v>
       </c>
-      <c r="O4" s="10">
-        <v>2.37</v>
-      </c>
-      <c r="P4" s="10">
-        <v>2.415</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>2.444</v>
-      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="9"/>
       <c r="R4" s="10">
         <v>1.89</v>
       </c>
@@ -4500,15 +4494,9 @@
         <f>H4*1.1</f>
         <v>3.7950000000000004</v>
       </c>
-      <c r="U4" s="13">
-        <v>2.915</v>
-      </c>
-      <c r="V4" s="13">
-        <v>2.988</v>
-      </c>
-      <c r="W4" s="12">
-        <v>3.3035999999999999</v>
-      </c>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="12"/>
       <c r="X4" s="13">
         <v>1.68</v>
       </c>
@@ -4519,15 +4507,9 @@
         <f>N4*1.1</f>
         <v>4.4660000000000002</v>
       </c>
-      <c r="AA4" s="10">
-        <v>2.37</v>
-      </c>
-      <c r="AB4" s="10">
-        <v>2.415</v>
-      </c>
-      <c r="AC4" s="9">
-        <v>2.444</v>
-      </c>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="9"/>
       <c r="AD4" s="10">
         <v>1.89</v>
       </c>
@@ -4538,15 +4520,9 @@
         <f>$H4*0.9</f>
         <v>3.1050000000000004</v>
       </c>
-      <c r="AG4" s="13">
-        <v>2.915</v>
-      </c>
-      <c r="AH4" s="12">
-        <v>3.3035999999999999</v>
-      </c>
-      <c r="AI4" s="13">
-        <v>2.988</v>
-      </c>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="13"/>
       <c r="AJ4" s="13">
         <v>1.68</v>
       </c>
@@ -4602,13 +4578,13 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="O5" s="17">
-        <v>1.716</v>
+        <v>1.597</v>
       </c>
       <c r="P5" s="17">
-        <v>1.7649999999999999</v>
+        <v>1.6419999999999999</v>
       </c>
       <c r="Q5" s="16">
-        <v>1.7969999999999999</v>
+        <v>1.673</v>
       </c>
       <c r="R5" s="17">
         <v>4.38</v>
@@ -4621,13 +4597,13 @@
         <v>5.2030000000000012</v>
       </c>
       <c r="U5" s="19">
-        <v>2.214</v>
+        <v>2.165</v>
       </c>
       <c r="V5" s="19">
-        <v>2.3050000000000002</v>
+        <v>2.2530000000000001</v>
       </c>
       <c r="W5" s="18">
-        <v>2.3660000000000001</v>
+        <v>2.3109999999999999</v>
       </c>
       <c r="X5" s="19">
         <v>1.9</v>
@@ -4639,15 +4615,9 @@
         <f>N5*1.1</f>
         <v>5.6210000000000004</v>
       </c>
-      <c r="AA5" s="17">
-        <v>1.716</v>
-      </c>
-      <c r="AB5" s="17">
-        <v>1.7649999999999999</v>
-      </c>
-      <c r="AC5" s="16">
-        <v>1.7969999999999999</v>
-      </c>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="16"/>
       <c r="AD5" s="17">
         <v>4.38</v>
       </c>
@@ -4658,15 +4628,9 @@
         <f t="shared" ref="AF5:AF8" si="0">$H5*0.9</f>
         <v>4.2570000000000006</v>
       </c>
-      <c r="AG5" s="19">
-        <v>2.214</v>
-      </c>
-      <c r="AH5" s="18">
-        <v>2.3660000000000001</v>
-      </c>
-      <c r="AI5" s="19">
-        <v>2.3050000000000002</v>
-      </c>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="19"/>
       <c r="AJ5" s="19">
         <v>1.9</v>
       </c>
@@ -4721,15 +4685,9 @@
       <c r="N6" s="20">
         <v>3.08</v>
       </c>
-      <c r="O6" s="17">
-        <v>1.643</v>
-      </c>
-      <c r="P6" s="17">
-        <v>1.6890000000000001</v>
-      </c>
-      <c r="Q6" s="16">
-        <v>1.7190000000000001</v>
-      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="16"/>
       <c r="R6" s="17">
         <v>23.38</v>
       </c>
@@ -4740,15 +4698,9 @@
         <f>H6*1.1</f>
         <v>4.7960000000000012</v>
       </c>
-      <c r="U6" s="19">
-        <v>2.2040000000000002</v>
-      </c>
-      <c r="V6" s="19">
-        <v>2.2890000000000001</v>
-      </c>
-      <c r="W6" s="18">
-        <v>2.3460000000000001</v>
-      </c>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="18"/>
       <c r="X6" s="19">
         <v>1.59</v>
       </c>
@@ -4759,15 +4711,9 @@
         <f>N6*1.1</f>
         <v>3.3880000000000003</v>
       </c>
-      <c r="AA6" s="17">
-        <v>1.643</v>
-      </c>
-      <c r="AB6" s="17">
-        <v>1.6890000000000001</v>
-      </c>
-      <c r="AC6" s="16">
-        <v>1.7190000000000001</v>
-      </c>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="16"/>
       <c r="AD6" s="17">
         <v>23.38</v>
       </c>
@@ -4778,15 +4724,9 @@
         <f t="shared" si="0"/>
         <v>3.9240000000000004</v>
       </c>
-      <c r="AG6" s="19">
-        <v>2.2040000000000002</v>
-      </c>
-      <c r="AH6" s="18">
-        <v>2.3460000000000001</v>
-      </c>
-      <c r="AI6" s="19">
-        <v>2.2890000000000001</v>
-      </c>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="19"/>
       <c r="AJ6" s="19">
         <v>1.59</v>
       </c>
@@ -4841,15 +4781,9 @@
       <c r="N7" s="20">
         <v>5.5</v>
       </c>
-      <c r="O7" s="17">
-        <v>2.238</v>
-      </c>
-      <c r="P7" s="17">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>2.274</v>
-      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="16"/>
       <c r="R7" s="17">
         <v>13.19</v>
       </c>
@@ -4860,15 +4794,9 @@
         <f>H7*1.1</f>
         <v>4.6640000000000006</v>
       </c>
-      <c r="U7" s="19">
-        <v>3.1509999999999998</v>
-      </c>
-      <c r="V7" s="19">
-        <v>3.2429999999999999</v>
-      </c>
-      <c r="W7" s="18">
-        <v>3.3039999999999998</v>
-      </c>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="18"/>
       <c r="X7" s="19">
         <v>2.56</v>
       </c>
@@ -4879,15 +4807,9 @@
         <f>N7*1.1</f>
         <v>6.0500000000000007</v>
       </c>
-      <c r="AA7" s="17">
-        <v>2.238</v>
-      </c>
-      <c r="AB7" s="17">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="AC7" s="16">
-        <v>2.274</v>
-      </c>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="16"/>
       <c r="AD7" s="17">
         <v>13.19</v>
       </c>
@@ -4898,15 +4820,9 @@
         <f t="shared" si="0"/>
         <v>3.8160000000000003</v>
       </c>
-      <c r="AG7" s="19">
-        <v>3.1509999999999998</v>
-      </c>
-      <c r="AH7" s="18">
-        <v>3.3039999999999998</v>
-      </c>
-      <c r="AI7" s="19">
-        <v>3.2429999999999999</v>
-      </c>
+      <c r="AG7" s="19"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="19"/>
       <c r="AJ7" s="19">
         <v>2.56</v>
       </c>
@@ -4961,15 +4877,9 @@
       <c r="N8" s="20">
         <v>3.22</v>
       </c>
-      <c r="O8" s="17">
-        <v>1.4770000000000001</v>
-      </c>
-      <c r="P8" s="17">
-        <v>1.5089999999999999</v>
-      </c>
-      <c r="Q8" s="16">
-        <v>1.5269999999999999</v>
-      </c>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="16"/>
       <c r="R8" s="17">
         <v>4.53</v>
       </c>
@@ -4980,15 +4890,9 @@
         <f>H8*1.1</f>
         <v>4.6970000000000001</v>
       </c>
-      <c r="U8" s="19">
-        <v>2.3769999999999998</v>
-      </c>
-      <c r="V8" s="19">
-        <v>2.476</v>
-      </c>
-      <c r="W8" s="18">
-        <v>2.5409999999999999</v>
-      </c>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="18"/>
       <c r="X8" s="19">
         <v>1.4</v>
       </c>
@@ -4999,15 +4903,9 @@
         <f>N8*1.1</f>
         <v>3.5420000000000007</v>
       </c>
-      <c r="AA8" s="17">
-        <v>1.4770000000000001</v>
-      </c>
-      <c r="AB8" s="17">
-        <v>1.5089999999999999</v>
-      </c>
-      <c r="AC8" s="16">
-        <v>1.5269999999999999</v>
-      </c>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="16"/>
       <c r="AD8" s="17">
         <v>4.53</v>
       </c>
@@ -5018,15 +4916,9 @@
         <f t="shared" si="0"/>
         <v>3.8429999999999995</v>
       </c>
-      <c r="AG8" s="19">
-        <v>2.3769999999999998</v>
-      </c>
-      <c r="AH8" s="18">
-        <v>2.5409999999999999</v>
-      </c>
-      <c r="AI8" s="19">
-        <v>2.476</v>
-      </c>
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="19"/>
       <c r="AJ8" s="19">
         <v>1.4</v>
       </c>

</xml_diff>

<commit_message>
fixed so mean dcew modified forecasting calculates correctly, updated new PET forcing files
</commit_message>
<xml_diff>
--- a/ClimateStatsforDCEW.xlsx
+++ b/ClimateStatsforDCEW.xlsx
@@ -597,11 +597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251005680"/>
-        <c:axId val="251005136"/>
+        <c:axId val="456306560"/>
+        <c:axId val="456309280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251005136"/>
+        <c:axId val="456309280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -623,7 +623,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -647,12 +646,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251005680"/>
+        <c:crossAx val="456306560"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251005680"/>
+        <c:axId val="456306560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,13 +673,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251005136"/>
+        <c:crossAx val="456309280"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -946,11 +944,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251010032"/>
-        <c:axId val="251014928"/>
+        <c:axId val="456311456"/>
+        <c:axId val="456307648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251014928"/>
+        <c:axId val="456307648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -972,7 +970,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -996,12 +993,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="251010032"/>
+        <c:crossAx val="456311456"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251010032"/>
+        <c:axId val="456311456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1023,13 +1020,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251014928"/>
+        <c:crossAx val="456307648"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1295,11 +1291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="415260880"/>
-        <c:axId val="415266320"/>
+        <c:axId val="456297856"/>
+        <c:axId val="456301664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="415266320"/>
+        <c:axId val="456301664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1317,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -1345,12 +1340,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415260880"/>
+        <c:crossAx val="456297856"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="415260880"/>
+        <c:axId val="456297856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,13 +1367,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="415266320"/>
+        <c:crossAx val="456301664"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1644,11 +1638,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="415270128"/>
-        <c:axId val="415258704"/>
+        <c:axId val="453873968"/>
+        <c:axId val="456309824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="415258704"/>
+        <c:axId val="456309824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,7 +1664,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -1694,12 +1687,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415270128"/>
+        <c:crossAx val="453873968"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="415270128"/>
+        <c:axId val="453873968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1721,13 +1714,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="415258704"/>
+        <c:crossAx val="456309824"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1993,11 +1985,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="415260336"/>
-        <c:axId val="415258160"/>
+        <c:axId val="494716976"/>
+        <c:axId val="494718064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="415258160"/>
+        <c:axId val="494718064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2019,7 +2011,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -2043,12 +2034,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415260336"/>
+        <c:crossAx val="494716976"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="415260336"/>
+        <c:axId val="494716976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2070,13 +2061,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="415258160"/>
+        <c:crossAx val="494718064"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2342,11 +2332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="415264144"/>
-        <c:axId val="415267408"/>
+        <c:axId val="494725136"/>
+        <c:axId val="494710448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="415267408"/>
+        <c:axId val="494710448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,7 +2358,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -2392,12 +2381,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415264144"/>
+        <c:crossAx val="494725136"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="415264144"/>
+        <c:axId val="494725136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2419,13 +2408,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="415267408"/>
+        <c:crossAx val="494710448"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3032,11 +3020,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="415265232"/>
-        <c:axId val="415263056"/>
+        <c:axId val="494712080"/>
+        <c:axId val="494719152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="415265232"/>
+        <c:axId val="494712080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,12 +3034,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="415263056"/>
+        <c:crossAx val="494719152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="415263056"/>
+        <c:axId val="494719152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.4"/>
@@ -3159,7 +3147,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="415265232"/>
+        <c:crossAx val="494712080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4240,10 +4228,10 @@
   <dimension ref="A1:AL8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X18" sqref="X18"/>
+      <selection pane="bottomRight" activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4422,11 +4410,11 @@
       <c r="AG3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AH3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI3" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="AI3" s="7" t="s">
-        <v>4</v>
       </c>
       <c r="AJ3" s="7" t="s">
         <v>5</v>
@@ -4521,8 +4509,8 @@
         <v>3.1050000000000004</v>
       </c>
       <c r="AG4" s="13"/>
-      <c r="AH4" s="12"/>
-      <c r="AI4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="12"/>
       <c r="AJ4" s="13">
         <v>1.68</v>
       </c>
@@ -4578,13 +4566,13 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="O5" s="17">
-        <v>1.597</v>
+        <v>1.863</v>
       </c>
       <c r="P5" s="17">
-        <v>1.6419999999999999</v>
+        <v>1.905</v>
       </c>
       <c r="Q5" s="16">
-        <v>1.673</v>
+        <v>1.9350000000000001</v>
       </c>
       <c r="R5" s="17">
         <v>4.38</v>
@@ -4597,13 +4585,13 @@
         <v>5.2030000000000012</v>
       </c>
       <c r="U5" s="19">
-        <v>2.165</v>
+        <v>2.3239999999999998</v>
       </c>
       <c r="V5" s="19">
-        <v>2.2530000000000001</v>
+        <v>2.4009999999999998</v>
       </c>
       <c r="W5" s="18">
-        <v>2.3109999999999999</v>
+        <v>2.452</v>
       </c>
       <c r="X5" s="19">
         <v>1.9</v>
@@ -4629,8 +4617,8 @@
         <v>4.2570000000000006</v>
       </c>
       <c r="AG5" s="19"/>
-      <c r="AH5" s="18"/>
-      <c r="AI5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="18"/>
       <c r="AJ5" s="19">
         <v>1.9</v>
       </c>

</xml_diff>

<commit_message>
updated MACA PET calculator, forcings txt files
</commit_message>
<xml_diff>
--- a/ClimateStatsforDCEW.xlsx
+++ b/ClimateStatsforDCEW.xlsx
@@ -64,13 +64,13 @@
     <t>BRW</t>
   </si>
   <si>
-    <t>decrease precipitation 10% depth</t>
-  </si>
-  <si>
     <t>Average temp and precip stats</t>
   </si>
   <si>
     <t>increase precipitation by 10% depth and temp with MACA R4.5 data</t>
+  </si>
+  <si>
+    <t>decrease precipitation 10% depth and temp with MAVA RCP4.5</t>
   </si>
 </sst>
 </file>
@@ -597,11 +597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="456306560"/>
-        <c:axId val="456309280"/>
+        <c:axId val="-1129957696"/>
+        <c:axId val="-1129958240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456309280"/>
+        <c:axId val="-1129958240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -646,12 +646,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456306560"/>
+        <c:crossAx val="-1129957696"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456306560"/>
+        <c:axId val="-1129957696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +678,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456309280"/>
+        <c:crossAx val="-1129958240"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -944,11 +944,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="456311456"/>
-        <c:axId val="456307648"/>
+        <c:axId val="-1090225536"/>
+        <c:axId val="-1334257440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456307648"/>
+        <c:axId val="-1334257440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,12 +993,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456311456"/>
+        <c:crossAx val="-1090225536"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456311456"/>
+        <c:axId val="-1090225536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1025,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456307648"/>
+        <c:crossAx val="-1334257440"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1291,11 +1291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="456297856"/>
-        <c:axId val="456301664"/>
+        <c:axId val="-1090218464"/>
+        <c:axId val="-1090220640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456301664"/>
+        <c:axId val="-1090220640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1340,12 +1340,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456297856"/>
+        <c:crossAx val="-1090218464"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456297856"/>
+        <c:axId val="-1090218464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1372,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456301664"/>
+        <c:crossAx val="-1090220640"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1542,7 +1542,7 @@
                   <c:v>2.444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7969999999999999</c:v>
+                  <c:v>1.8620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.7190000000000001</c:v>
@@ -1614,7 +1614,7 @@
                   <c:v>3.3035999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3660000000000001</c:v>
+                  <c:v>2.5009999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.3460000000000001</c:v>
@@ -1638,11 +1638,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="453873968"/>
-        <c:axId val="456309824"/>
+        <c:axId val="-1090223360"/>
+        <c:axId val="-1090217376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456309824"/>
+        <c:axId val="-1090217376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1687,12 +1687,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453873968"/>
+        <c:crossAx val="-1090223360"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="453873968"/>
+        <c:axId val="-1090223360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1719,7 +1719,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456309824"/>
+        <c:crossAx val="-1090217376"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1889,7 +1889,7 @@
                   <c:v>2.37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.716</c:v>
+                  <c:v>1.7769999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.643</c:v>
@@ -1961,7 +1961,7 @@
                   <c:v>2.915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.214</c:v>
+                  <c:v>2.3450000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.2040000000000002</c:v>
@@ -1985,11 +1985,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="494716976"/>
-        <c:axId val="494718064"/>
+        <c:axId val="-1090217920"/>
+        <c:axId val="-1090212480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494718064"/>
+        <c:axId val="-1090212480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2034,12 +2034,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494716976"/>
+        <c:crossAx val="-1090217920"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494716976"/>
+        <c:axId val="-1090217920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2066,7 +2066,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494718064"/>
+        <c:crossAx val="-1090212480"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2236,7 +2236,7 @@
                   <c:v>2.415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7649999999999999</c:v>
+                  <c:v>1.8280000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.6890000000000001</c:v>
@@ -2308,7 +2308,7 @@
                   <c:v>2.988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3050000000000002</c:v>
+                  <c:v>2.4390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.2890000000000001</c:v>
@@ -2332,11 +2332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="494725136"/>
-        <c:axId val="494710448"/>
+        <c:axId val="-1090226080"/>
+        <c:axId val="-1090215744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494710448"/>
+        <c:axId val="-1090215744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2381,12 +2381,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494725136"/>
+        <c:crossAx val="-1090226080"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494725136"/>
+        <c:axId val="-1090226080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2413,7 +2413,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494710448"/>
+        <c:crossAx val="-1090215744"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2571,7 +2571,7 @@
                   <c:v>2.37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.716</c:v>
+                  <c:v>1.7769999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.643</c:v>
@@ -2656,7 +2656,7 @@
                   <c:v>2.415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7649999999999999</c:v>
+                  <c:v>1.8280000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.6890000000000001</c:v>
@@ -2741,7 +2741,7 @@
                   <c:v>2.444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7969999999999999</c:v>
+                  <c:v>1.8620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.7190000000000001</c:v>
@@ -2826,7 +2826,7 @@
                   <c:v>2.915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.214</c:v>
+                  <c:v>2.3450000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.2040000000000002</c:v>
@@ -2911,7 +2911,7 @@
                   <c:v>2.988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3050000000000002</c:v>
+                  <c:v>2.4390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.2890000000000001</c:v>
@@ -2996,7 +2996,7 @@
                   <c:v>3.3035999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3660000000000001</c:v>
+                  <c:v>2.5009999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.3460000000000001</c:v>
@@ -3020,11 +3020,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="494712080"/>
-        <c:axId val="494719152"/>
+        <c:axId val="-1090211936"/>
+        <c:axId val="-1090211392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494712080"/>
+        <c:axId val="-1090211936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3034,12 +3034,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494719152"/>
+        <c:crossAx val="-1090211392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494719152"/>
+        <c:axId val="-1090211392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.4"/>
@@ -3147,7 +3147,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494712080"/>
+        <c:crossAx val="-1090211936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4228,10 +4228,10 @@
   <dimension ref="A1:AL8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD19" sqref="AD19"/>
+      <selection pane="bottomRight" activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4275,12 +4275,12 @@
   <sheetData>
     <row r="1" spans="1:38">
       <c r="C1" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="O1" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
@@ -4288,7 +4288,7 @@
       <c r="S1" s="22"/>
       <c r="T1" s="22"/>
       <c r="AA1" s="22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AB1" s="22"/>
       <c r="AC1" s="22"/>
@@ -4530,13 +4530,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="17">
-        <v>1.716</v>
+        <v>1.7769999999999999</v>
       </c>
       <c r="D5" s="17">
-        <v>1.7649999999999999</v>
+        <v>1.8280000000000001</v>
       </c>
       <c r="E5" s="16">
-        <v>1.7969999999999999</v>
+        <v>1.8620000000000001</v>
       </c>
       <c r="F5" s="17">
         <v>4.38</v>
@@ -4548,13 +4548,13 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="I5" s="19">
-        <v>2.214</v>
+        <v>2.3450000000000002</v>
       </c>
       <c r="J5" s="19">
-        <v>2.3050000000000002</v>
+        <v>2.4390000000000001</v>
       </c>
       <c r="K5" s="18">
-        <v>2.3660000000000001</v>
+        <v>2.5009999999999999</v>
       </c>
       <c r="L5" s="19">
         <v>1.9</v>
@@ -4566,13 +4566,13 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="O5" s="17">
-        <v>1.863</v>
+        <v>1.871</v>
       </c>
       <c r="P5" s="17">
-        <v>1.905</v>
+        <v>1.9239999999999999</v>
       </c>
       <c r="Q5" s="16">
-        <v>1.9350000000000001</v>
+        <v>1.9590000000000001</v>
       </c>
       <c r="R5" s="17">
         <v>4.38</v>
@@ -4585,13 +4585,13 @@
         <v>5.2030000000000012</v>
       </c>
       <c r="U5" s="19">
-        <v>2.3239999999999998</v>
+        <v>2.4980000000000002</v>
       </c>
       <c r="V5" s="19">
-        <v>2.4009999999999998</v>
+        <v>2.5979999999999999</v>
       </c>
       <c r="W5" s="18">
-        <v>2.452</v>
+        <v>2.665</v>
       </c>
       <c r="X5" s="19">
         <v>1.9</v>
@@ -4603,9 +4603,15 @@
         <f>N5*1.1</f>
         <v>5.6210000000000004</v>
       </c>
-      <c r="AA5" s="17"/>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="16"/>
+      <c r="AA5" s="17">
+        <v>1.6859999999999999</v>
+      </c>
+      <c r="AB5" s="17">
+        <v>1.736</v>
+      </c>
+      <c r="AC5" s="16">
+        <v>1.766</v>
+      </c>
       <c r="AD5" s="17">
         <v>4.38</v>
       </c>
@@ -4616,9 +4622,15 @@
         <f t="shared" ref="AF5:AF8" si="0">$H5*0.9</f>
         <v>4.2570000000000006</v>
       </c>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="18"/>
+      <c r="AG5" s="19">
+        <v>2.2010000000000001</v>
+      </c>
+      <c r="AH5" s="19">
+        <v>2.2890000000000001</v>
+      </c>
+      <c r="AI5" s="18">
+        <v>2.3479999999999999</v>
+      </c>
       <c r="AJ5" s="19">
         <v>1.9</v>
       </c>

</xml_diff>

<commit_message>
updated weather station climate stats graphs
</commit_message>
<xml_diff>
--- a/ClimateStatsforDCEW.xlsx
+++ b/ClimateStatsforDCEW.xlsx
@@ -444,7 +444,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -475,7 +475,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -484,7 +483,62 @@
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -907,11 +961,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1839608480"/>
-        <c:axId val="1839609024"/>
+        <c:axId val="-1152861328"/>
+        <c:axId val="-888078224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1839608480"/>
+        <c:axId val="-1152861328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,12 +1008,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839609024"/>
+        <c:crossAx val="-888078224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1839609024"/>
+        <c:axId val="-888078224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.75"/>
@@ -1004,7 +1058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1839608480"/>
+        <c:crossAx val="-1152861328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1601,11 +1655,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1889616112"/>
-        <c:axId val="1889614480"/>
+        <c:axId val="-885191392"/>
+        <c:axId val="-885196832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1889616112"/>
+        <c:axId val="-885191392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,12 +1669,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1889614480"/>
+        <c:crossAx val="-885196832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1889614480"/>
+        <c:axId val="-885196832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.4"/>
@@ -1728,7 +1782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1889616112"/>
+        <c:crossAx val="-885191392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2193,11 +2247,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1799588928"/>
-        <c:axId val="1597066272"/>
+        <c:axId val="-888075504"/>
+        <c:axId val="-888079856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1799588928"/>
+        <c:axId val="-888075504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,12 +2294,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1597066272"/>
+        <c:crossAx val="-888079856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1597066272"/>
+        <c:axId val="-888079856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2288,7 +2342,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1799588928"/>
+        <c:crossAx val="-888075504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2497,11 +2551,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1888528944"/>
-        <c:axId val="1888520240"/>
+        <c:axId val="-888073872"/>
+        <c:axId val="-888079312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1888528944"/>
+        <c:axId val="-888073872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2544,12 +2598,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888520240"/>
+        <c:crossAx val="-888079312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1888520240"/>
+        <c:axId val="-888079312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2592,7 +2646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888528944"/>
+        <c:crossAx val="-888073872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2848,11 +2902,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1888527312"/>
-        <c:axId val="1888513712"/>
+        <c:axId val="-888068432"/>
+        <c:axId val="-888077680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1888513712"/>
+        <c:axId val="-888077680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2897,12 +2951,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888527312"/>
+        <c:crossAx val="-888068432"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1888527312"/>
+        <c:axId val="-888068432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2929,7 +2983,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888513712"/>
+        <c:crossAx val="-888077680"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3195,11 +3249,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1888527856"/>
-        <c:axId val="1888528400"/>
+        <c:axId val="-888076592"/>
+        <c:axId val="-888080944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1888528400"/>
+        <c:axId val="-888080944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3244,12 +3298,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888527856"/>
+        <c:crossAx val="-888076592"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1888527856"/>
+        <c:axId val="-888076592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3276,7 +3330,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888528400"/>
+        <c:crossAx val="-888080944"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3542,11 +3596,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1888526768"/>
-        <c:axId val="1888525680"/>
+        <c:axId val="-888074416"/>
+        <c:axId val="-888072784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1888525680"/>
+        <c:axId val="-888072784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3591,12 +3645,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888526768"/>
+        <c:crossAx val="-888074416"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1888526768"/>
+        <c:axId val="-888074416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3623,7 +3677,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888525680"/>
+        <c:crossAx val="-888072784"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3889,11 +3943,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1888522416"/>
-        <c:axId val="1888515888"/>
+        <c:axId val="-888074960"/>
+        <c:axId val="-888082576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1888515888"/>
+        <c:axId val="-888082576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3938,12 +3992,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888522416"/>
+        <c:crossAx val="-888074960"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1888522416"/>
+        <c:axId val="-888074960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,7 +4024,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888515888"/>
+        <c:crossAx val="-888082576"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4236,11 +4290,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1888523504"/>
-        <c:axId val="1888522960"/>
+        <c:axId val="-888070608"/>
+        <c:axId val="-888071152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1888522960"/>
+        <c:axId val="-888071152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4285,12 +4339,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888523504"/>
+        <c:crossAx val="-888070608"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1888523504"/>
+        <c:axId val="-888070608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4317,7 +4371,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888522960"/>
+        <c:crossAx val="-888071152"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4583,11 +4637,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1888524048"/>
-        <c:axId val="1888521328"/>
+        <c:axId val="-885198464"/>
+        <c:axId val="-885197376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1888521328"/>
+        <c:axId val="-885197376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4632,12 +4686,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1888524048"/>
+        <c:crossAx val="-885198464"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1888524048"/>
+        <c:axId val="-885198464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4664,7 +4718,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1888521328"/>
+        <c:crossAx val="-885197376"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8588,8 +8642,125 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A19:C23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisPage" showAll="0">
+      <items count="11">
+        <item m="1" x="5"/>
+        <item m="1" x="9"/>
+        <item m="1" x="7"/>
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item m="1" x="5"/>
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item m="1" x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="0" item="6" hier="-1"/>
+    <pageField fld="4" item="2" hier="-1"/>
+    <pageField fld="1" item="0" hier="-1"/>
+    <pageField fld="2" item="4" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="16">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A6:C10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <location ref="A7:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisPage" showAll="0">
       <items count="11">
@@ -8684,12 +8855,17 @@
   <pageFields count="4">
     <pageField fld="0" item="6" hier="-1"/>
     <pageField fld="4" item="0" hier="-1"/>
-    <pageField fld="1" item="3" hier="-1"/>
+    <pageField fld="1" item="5" hier="-1"/>
     <pageField fld="2" item="4" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0"/>
+    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
   </dataFields>
+  <formats count="1">
+    <format dxfId="17">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -8699,9 +8875,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E18:G22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <location ref="E19:G23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisPage" showAll="0">
       <items count="11">
@@ -8800,8 +8976,13 @@
     <pageField fld="2" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0"/>
+    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
   </dataFields>
+  <formats count="1">
+    <format dxfId="10">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -8811,9 +8992,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E6:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <location ref="E7:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisPage" showAll="0">
       <items count="11">
@@ -8908,124 +9089,17 @@
   <pageFields count="4">
     <pageField fld="0" item="6" hier="-1"/>
     <pageField fld="4" item="0" hier="-1"/>
-    <pageField fld="1" item="5" hier="-1"/>
-    <pageField fld="2" item="4" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A18:C22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="7">
-    <pivotField axis="axisPage" showAll="0">
-      <items count="11">
-        <item m="1" x="5"/>
-        <item m="1" x="9"/>
-        <item m="1" x="7"/>
-        <item m="1" x="6"/>
-        <item m="1" x="8"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item m="1" x="5"/>
-        <item m="1" x="4"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item m="1" x="5"/>
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item m="1" x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="3"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="4">
-    <pageField fld="0" item="6" hier="-1"/>
-    <pageField fld="4" item="2" hier="-1"/>
-    <pageField fld="1" item="0" hier="-1"/>
+    <pageField fld="1" item="3" hier="-1"/>
     <pageField fld="2" item="5" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0"/>
+    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
   </dataFields>
+  <formats count="1">
+    <format dxfId="11">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -13581,321 +13655,321 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="3" max="3" width="5.375" customWidth="1"/>
     <col min="4" max="4" width="3.5" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.125" customWidth="1"/>
-    <col min="7" max="7" width="5.875" customWidth="1"/>
+    <col min="7" max="7" width="4.375" customWidth="1"/>
     <col min="8" max="8" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="2" spans="1:7">
       <c r="A2" s="24" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="24" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>33</v>
+      <c r="F5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="26">
-        <v>2.4980000000000002</v>
-      </c>
-      <c r="C8" s="26">
-        <v>1.871</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="26">
-        <v>2.5990000000000002</v>
-      </c>
-      <c r="G8" s="26">
-        <v>1.921</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="26">
-        <v>2.5979999999999999</v>
-      </c>
-      <c r="C9" s="26">
-        <v>1.9239999999999999</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.5990000000000002</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.921</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="26">
-        <v>2.7719999999999998</v>
-      </c>
-      <c r="G9" s="26">
-        <v>1.9770000000000001</v>
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.2010000000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.6859999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.7719999999999998</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.2890000000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.736</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="26">
-        <v>2.665</v>
-      </c>
-      <c r="C10" s="26">
-        <v>1.9590000000000001</v>
-      </c>
-      <c r="E10" s="25" t="s">
+      <c r="B11" s="2">
+        <v>2.7029999999999998</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.012</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="26">
-        <v>2.7029999999999998</v>
-      </c>
-      <c r="G10" s="26">
-        <v>2.012</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
+      <c r="F11" s="2">
+        <v>2.3479999999999999</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.766</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="24" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="24" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="24" t="s">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E20" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>1</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="26">
-        <v>4.5990000000000002</v>
-      </c>
-      <c r="C20" s="26">
-        <v>4.2570000000000006</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="26">
-        <v>2.214</v>
-      </c>
-      <c r="G20" s="26">
-        <v>1.716</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="26">
-        <v>365.15</v>
-      </c>
-      <c r="C21" s="26">
-        <v>71.41</v>
+        <v>31</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5.6210000000000004</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5.2030000000000012</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="26">
-        <v>2.3050000000000002</v>
-      </c>
-      <c r="G21" s="26">
-        <v>1.7649999999999999</v>
+        <v>3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2.214</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.716</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2">
+        <v>365.15</v>
+      </c>
+      <c r="C22" s="2">
+        <v>71.41</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="2">
+        <v>2.3050000000000002</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.7649999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B23" s="2">
         <v>1.9</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C23" s="2">
         <v>4.38</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E23" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F23" s="2">
         <v>2.3660000000000001</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G23" s="2">
         <v>1.7969999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made it easier to get descriptive statistics
</commit_message>
<xml_diff>
--- a/ClimateStatsforDCEW.xlsx
+++ b/ClimateStatsforDCEW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" tabRatio="657" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" tabRatio="657" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Pivot Table" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="52">
   <si>
     <t>wet</t>
   </si>
@@ -173,11 +173,20 @@
   <si>
     <t>Bogus Ridge Weather</t>
   </si>
+  <si>
+    <t>Treeline 4.5</t>
+  </si>
+  <si>
+    <t>Treeline 8.5</t>
+  </si>
+  <si>
+    <t>T average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -483,49 +492,7 @@
     <cellStyle name="Result" xfId="3"/>
     <cellStyle name="Result2" xfId="4"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -552,7 +519,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -641,6 +608,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5DB2-4F68-AE47-8D6C15FAA3DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -702,6 +674,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5DB2-4F68-AE47-8D6C15FAA3DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -766,6 +743,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5DB2-4F68-AE47-8D6C15FAA3DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -827,6 +809,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5DB2-4F68-AE47-8D6C15FAA3DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -888,6 +875,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5DB2-4F68-AE47-8D6C15FAA3DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -952,6 +944,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5DB2-4F68-AE47-8D6C15FAA3DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1108,7 +1105,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1221,6 +1218,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AF45-409E-A1BD-C07CAEB4B10A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1306,6 +1308,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AF45-409E-A1BD-C07CAEB4B10A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1391,6 +1398,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AF45-409E-A1BD-C07CAEB4B10A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1476,6 +1488,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AF45-409E-A1BD-C07CAEB4B10A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1561,6 +1578,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AF45-409E-A1BD-C07CAEB4B10A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -1646,6 +1668,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-AF45-409E-A1BD-C07CAEB4B10A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1873,7 +1900,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1985,6 +2012,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AEE4-4365-9C52-751B7A277825}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2048,6 +2080,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AEE4-4365-9C52-751B7A277825}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2111,6 +2148,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AEE4-4365-9C52-751B7A277825}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -2175,6 +2217,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AEE4-4365-9C52-751B7A277825}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2238,6 +2285,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AEE4-4365-9C52-751B7A277825}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2392,7 +2444,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2481,6 +2533,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C91C-43BD-9FE0-FBE5DD947158}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -2542,6 +2599,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C91C-43BD-9FE0-FBE5DD947158}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2696,7 +2758,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2821,6 +2883,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-440E-4A0D-9682-FA48D858505D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2893,6 +2960,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-440E-4A0D-9682-FA48D858505D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3043,7 +3115,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3168,6 +3240,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C45F-4BC5-883B-9B3B5430EAA6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3240,6 +3317,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C45F-4BC5-883B-9B3B5430EAA6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3390,7 +3472,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3515,6 +3597,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4423-44EC-A908-0D90627A10BD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3587,6 +3674,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4423-44EC-A908-0D90627A10BD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3737,7 +3829,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3862,6 +3954,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E1CB-4F82-82C0-1E08947801BC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3934,6 +4031,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E1CB-4F82-82C0-1E08947801BC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4084,7 +4186,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4209,6 +4311,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F164-4E9A-AB7B-1B9EBA1A368E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4281,6 +4388,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F164-4E9A-AB7B-1B9EBA1A368E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4431,7 +4543,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4556,6 +4668,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E57-47EE-890D-C68465C9D51C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4628,6 +4745,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E57-47EE-890D-C68465C9D51C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7018,7 +7140,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7048,7 +7176,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7078,7 +7212,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7103,7 +7243,13 @@
     <xdr:ext cx="5416931" cy="3241421"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7125,7 +7271,13 @@
     <xdr:ext cx="5416931" cy="3241421"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7147,7 +7299,13 @@
     <xdr:ext cx="5416931" cy="3241421"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7169,7 +7327,13 @@
     <xdr:ext cx="5416931" cy="3241421"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7191,7 +7355,13 @@
     <xdr:ext cx="5416931" cy="3241421"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7213,7 +7383,13 @@
     <xdr:ext cx="5416931" cy="3241421"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7245,7 +7421,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -7268,7 +7450,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Lucy Gelb" refreshedDate="42436.598321874997" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="144">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:G146" sheet="Sheet1"/>
+    <worksheetSource ref="A1:G145" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Weather Station" numFmtId="0">
@@ -8642,6 +8824,240 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E19:G23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisPage" showAll="0">
+      <items count="11">
+        <item m="1" x="5"/>
+        <item m="1" x="9"/>
+        <item m="1" x="7"/>
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item m="1" x="5"/>
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item m="1" x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="0" item="6" hier="-1"/>
+    <pageField fld="4" item="0" hier="-1"/>
+    <pageField fld="1" item="4" hier="-1"/>
+    <pageField fld="2" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E7:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisPage" showAll="0">
+      <items count="11">
+        <item m="1" x="5"/>
+        <item m="1" x="9"/>
+        <item m="1" x="7"/>
+        <item m="1" x="6"/>
+        <item m="1" x="8"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="1"/>
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item m="1" x="5"/>
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item m="1" x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="0" item="6" hier="-1"/>
+    <pageField fld="4" item="0" hier="-1"/>
+    <pageField fld="1" item="3" hier="-1"/>
+    <pageField fld="2" item="5" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="7">
@@ -8745,7 +9161,7 @@
     <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="16">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -8758,7 +9174,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:C11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="7">
@@ -8862,241 +9278,7 @@
     <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="17">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E19:G23" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="7">
-    <pivotField axis="axisPage" showAll="0">
-      <items count="11">
-        <item m="1" x="5"/>
-        <item m="1" x="9"/>
-        <item m="1" x="7"/>
-        <item m="1" x="6"/>
-        <item m="1" x="8"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item m="1" x="5"/>
-        <item m="1" x="4"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item m="1" x="5"/>
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item m="1" x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="3"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="4">
-    <pageField fld="0" item="6" hier="-1"/>
-    <pageField fld="4" item="0" hier="-1"/>
-    <pageField fld="1" item="4" hier="-1"/>
-    <pageField fld="2" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="10">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E7:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="7">
-    <pivotField axis="axisPage" showAll="0">
-      <items count="11">
-        <item m="1" x="5"/>
-        <item m="1" x="9"/>
-        <item m="1" x="7"/>
-        <item m="1" x="6"/>
-        <item m="1" x="8"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="1"/>
-        <item m="1" x="5"/>
-        <item m="1" x="4"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item m="1" x="5"/>
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item m="1" x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="3"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="4">
-    <pageField fld="0" item="6" hier="-1"/>
-    <pageField fld="4" item="0" hier="-1"/>
-    <pageField fld="1" item="3" hier="-1"/>
-    <pageField fld="2" item="5" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Average of value" fld="6" subtotal="average" baseField="5" baseItem="0" numFmtId="2"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="11">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -9185,6 +9367,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9220,6 +9419,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9375,10 +9591,10 @@
   <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="X29" sqref="S25:X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10077,6 +10293,26 @@
         <v>2.8980000000000001</v>
       </c>
     </row>
+    <row r="11" spans="1:38">
+      <c r="S11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="W11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
         <v>20</v>
@@ -10108,6 +10344,33 @@
       <c r="K12" s="19">
         <v>4.5990000000000002</v>
       </c>
+      <c r="R12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S12" s="2">
+        <f>O5/C5</f>
+        <v>1.0903263403263403</v>
+      </c>
+      <c r="T12" s="2">
+        <f>P5/D5</f>
+        <v>1.090084985835694</v>
+      </c>
+      <c r="U12" s="2">
+        <f t="shared" ref="T12:U12" si="2">Q5/E5</f>
+        <v>1.0901502504173624</v>
+      </c>
+      <c r="V12" s="2">
+        <f>U5/I5</f>
+        <v>1.1282746160794943</v>
+      </c>
+      <c r="W12" s="2">
+        <f t="shared" ref="W12:X12" si="3">V5/J5</f>
+        <v>1.1271149674620389</v>
+      </c>
+      <c r="X12" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1263736263736264</v>
+      </c>
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
@@ -10140,6 +10403,33 @@
       <c r="K13" s="19">
         <v>5.1100000000000003</v>
       </c>
+      <c r="R13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S13" s="2">
+        <f>AA5/C5</f>
+        <v>0.9825174825174825</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" ref="T13:U13" si="4">AB5/D5</f>
+        <v>0.98356940509915014</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.98274902615470228</v>
+      </c>
+      <c r="V13" s="2">
+        <f>AG5/I5</f>
+        <v>0.99412827461607955</v>
+      </c>
+      <c r="W13" s="2">
+        <f t="shared" ref="W13:X13" si="5">AH5/J5</f>
+        <v>0.99305856832971795</v>
+      </c>
+      <c r="X13" s="2">
+        <f t="shared" si="5"/>
+        <v>0.99239222316145381</v>
+      </c>
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
@@ -10177,7 +10467,7 @@
       <c r="A15" s="2"/>
       <c r="P15" s="15"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:24">
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -10187,8 +10477,29 @@
       <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="R17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S17" s="17">
+        <v>1.716</v>
+      </c>
+      <c r="T17" s="17">
+        <v>1.7649999999999999</v>
+      </c>
+      <c r="U17" s="16">
+        <v>1.7969999999999999</v>
+      </c>
+      <c r="V17" s="19">
+        <v>2.214</v>
+      </c>
+      <c r="W17" s="19">
+        <v>2.3050000000000002</v>
+      </c>
+      <c r="X17" s="18">
+        <v>2.3660000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -10210,8 +10521,29 @@
       <c r="G18" s="19">
         <v>2.2010000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="R18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S18" s="17">
+        <v>1.871</v>
+      </c>
+      <c r="T18" s="17">
+        <v>1.9239999999999999</v>
+      </c>
+      <c r="U18" s="16">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="V18" s="19">
+        <v>2.4980000000000002</v>
+      </c>
+      <c r="W18" s="19">
+        <v>2.5979999999999999</v>
+      </c>
+      <c r="X18" s="18">
+        <v>2.665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -10236,8 +10568,29 @@
       <c r="L19" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="R19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S19" s="17">
+        <v>1.6859999999999999</v>
+      </c>
+      <c r="T19" s="17">
+        <v>1.736</v>
+      </c>
+      <c r="U19" s="16">
+        <v>1.766</v>
+      </c>
+      <c r="V19" s="19">
+        <v>2.2010000000000001</v>
+      </c>
+      <c r="W19" s="19">
+        <v>2.2890000000000001</v>
+      </c>
+      <c r="X19" s="18">
+        <v>2.3479999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -10275,7 +10628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="O47"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
@@ -10294,10 +10647,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G146"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C122" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10312,27 +10666,50 @@
     <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="23" customFormat="1" ht="15">
-      <c r="A2" s="23" t="s">
+    <row r="1" spans="1:7" s="23" customFormat="1" ht="15">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>2.37</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -10352,10 +10729,10 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>2.37</v>
+        <v>2.415</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -10375,10 +10752,10 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>2.415</v>
+        <v>2.444</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -10392,16 +10769,16 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>2.444</v>
+        <v>2.915</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -10421,10 +10798,10 @@
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>2.915</v>
+        <v>2.988</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -10444,10 +10821,10 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>2.988</v>
+        <v>3.036</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -10461,16 +10838,16 @@
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G8">
-        <v>3.036</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -10490,10 +10867,10 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9">
-        <v>1.89</v>
+        <v>104.92</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -10513,10 +10890,10 @@
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G10">
-        <v>104.92</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -10530,16 +10907,16 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G11">
-        <v>3.45</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -10559,10 +10936,10 @@
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G12">
-        <v>1.68</v>
+        <v>505.82</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -10582,15 +10959,15 @@
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G13">
-        <v>505.82</v>
+        <v>4.0599999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -10599,16 +10976,16 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>4.0599999999999996</v>
+        <v>1.716</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -10628,10 +11005,10 @@
         <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>1.716</v>
+        <v>1.7649999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -10651,10 +11028,10 @@
         <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>1.7649999999999999</v>
+        <v>1.7969999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -10671,13 +11048,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G17">
-        <v>1.7969999999999999</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -10697,10 +11074,10 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G18">
-        <v>4.38</v>
+        <v>71.41</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -10720,10 +11097,10 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G19">
-        <v>71.41</v>
+        <v>4.7300000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -10737,16 +11114,16 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G20">
-        <v>4.7300000000000004</v>
+        <v>2.214</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -10766,10 +11143,10 @@
         <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21">
-        <v>2.214</v>
+        <v>2.3050000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -10789,10 +11166,10 @@
         <v>26</v>
       </c>
       <c r="F22" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>2.3050000000000002</v>
+        <v>2.3660000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -10809,13 +11186,13 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G23">
-        <v>2.3660000000000001</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -10835,10 +11212,10 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G24">
-        <v>1.9</v>
+        <v>365.15</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -10858,15 +11235,15 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G25">
-        <v>365.15</v>
+        <v>5.1100000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -10875,16 +11252,16 @@
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G26">
-        <v>5.1100000000000003</v>
+        <v>1.643</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -10904,10 +11281,10 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>1.643</v>
+        <v>1.6890000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -10927,10 +11304,10 @@
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <v>1.6890000000000001</v>
+        <v>1.7190000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -10947,13 +11324,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G29">
-        <v>1.7190000000000001</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -10973,10 +11350,10 @@
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G30">
-        <v>23.38</v>
+        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -10996,10 +11373,10 @@
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G31">
-        <v>66.400000000000006</v>
+        <v>4.3600000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -11013,16 +11390,16 @@
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G32">
-        <v>4.3600000000000003</v>
+        <v>2.2040000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -11042,10 +11419,10 @@
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G33">
-        <v>2.2040000000000002</v>
+        <v>2.2890000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -11065,10 +11442,10 @@
         <v>26</v>
       </c>
       <c r="F34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>2.2890000000000001</v>
+        <v>2.3460000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -11085,13 +11462,13 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G35">
-        <v>2.3460000000000001</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -11111,10 +11488,10 @@
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G36">
-        <v>1.59</v>
+        <v>191.67</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -11134,15 +11511,15 @@
         <v>43</v>
       </c>
       <c r="F37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G37">
-        <v>191.67</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -11151,16 +11528,16 @@
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F38" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G38">
-        <v>3.08</v>
+        <v>2.238</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -11180,10 +11557,10 @@
         <v>26</v>
       </c>
       <c r="F39" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G39">
-        <v>2.238</v>
+        <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -11203,10 +11580,10 @@
         <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G40">
-        <v>2.2599999999999998</v>
+        <v>2.274</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -11223,13 +11600,13 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G41">
-        <v>2.274</v>
+        <v>13.19</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -11249,10 +11626,10 @@
         <v>43</v>
       </c>
       <c r="F42" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G42">
-        <v>13.19</v>
+        <v>79.209999999999994</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -11272,10 +11649,10 @@
         <v>43</v>
       </c>
       <c r="F43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G43">
-        <v>79.209999999999994</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -11289,16 +11666,16 @@
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G44">
-        <v>4.24</v>
+        <v>3.1509999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -11318,10 +11695,10 @@
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G45">
-        <v>3.1509999999999998</v>
+        <v>3.2429999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -11341,10 +11718,10 @@
         <v>26</v>
       </c>
       <c r="F46" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G46">
-        <v>3.2429999999999999</v>
+        <v>3.3039999999999998</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -11361,13 +11738,13 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F47" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G47">
-        <v>3.3039999999999998</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -11387,10 +11764,10 @@
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G48">
-        <v>2.56</v>
+        <v>377.28</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -11410,15 +11787,15 @@
         <v>43</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G49">
-        <v>377.28</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -11427,16 +11804,16 @@
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G50">
-        <v>5.5</v>
+        <v>1.4770000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -11456,10 +11833,10 @@
         <v>26</v>
       </c>
       <c r="F51" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>1.4770000000000001</v>
+        <v>1.5089999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -11479,10 +11856,10 @@
         <v>26</v>
       </c>
       <c r="F52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G52">
-        <v>1.5089999999999999</v>
+        <v>1.5269999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -11499,13 +11876,13 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F53" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G53">
-        <v>1.5269999999999999</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -11525,10 +11902,10 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G54">
-        <v>4.53</v>
+        <v>56.32</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -11548,10 +11925,10 @@
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G55">
-        <v>56.32</v>
+        <v>4.2699999999999996</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -11565,16 +11942,16 @@
         <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G56">
-        <v>4.2699999999999996</v>
+        <v>2.3769999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -11594,10 +11971,10 @@
         <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G57">
-        <v>2.3769999999999998</v>
+        <v>2.476</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -11617,10 +11994,10 @@
         <v>26</v>
       </c>
       <c r="F58" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G58">
-        <v>2.476</v>
+        <v>2.5409999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -11637,13 +12014,13 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F59" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G59">
-        <v>2.5409999999999999</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -11663,10 +12040,10 @@
         <v>43</v>
       </c>
       <c r="F60" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G60">
-        <v>1.4</v>
+        <v>192.71</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -11686,33 +12063,33 @@
         <v>43</v>
       </c>
       <c r="F61" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G61">
-        <v>192.71</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" t="s">
         <v>43</v>
       </c>
       <c r="F62" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G62">
-        <v>3.22</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -11732,10 +12109,10 @@
         <v>43</v>
       </c>
       <c r="F63" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G63">
-        <v>4.38</v>
+        <v>71.41</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -11755,10 +12132,10 @@
         <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G64">
-        <v>71.41</v>
+        <v>5.2030000000000012</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -11772,16 +12149,16 @@
         <v>40</v>
       </c>
       <c r="D65" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" t="s">
         <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G65">
-        <v>5.2030000000000012</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -11801,10 +12178,10 @@
         <v>43</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G66">
-        <v>1.9</v>
+        <v>365.15</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -11824,10 +12201,10 @@
         <v>43</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G67">
-        <v>365.15</v>
+        <v>5.6210000000000004</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -11838,19 +12215,19 @@
         <v>39</v>
       </c>
       <c r="C68" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" t="s">
         <v>43</v>
       </c>
       <c r="F68" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G68">
-        <v>5.6210000000000004</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -11870,10 +12247,10 @@
         <v>43</v>
       </c>
       <c r="F69" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G69">
-        <v>4.38</v>
+        <v>71.41</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -11893,10 +12270,10 @@
         <v>43</v>
       </c>
       <c r="F70" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G70">
-        <v>71.41</v>
+        <v>4.2570000000000006</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -11910,16 +12287,16 @@
         <v>41</v>
       </c>
       <c r="D71" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
         <v>43</v>
       </c>
       <c r="F71" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G71">
-        <v>4.2570000000000006</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -11939,10 +12316,10 @@
         <v>43</v>
       </c>
       <c r="F72" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G72">
-        <v>1.9</v>
+        <v>365.15</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -11962,10 +12339,10 @@
         <v>43</v>
       </c>
       <c r="F73" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G73">
-        <v>365.15</v>
+        <v>4.5990000000000002</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -11973,22 +12350,22 @@
         <v>45</v>
       </c>
       <c r="B74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C74" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F74" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G74">
-        <v>4.5990000000000002</v>
+        <v>1.871</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -12008,10 +12385,10 @@
         <v>26</v>
       </c>
       <c r="F75" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G75">
-        <v>1.871</v>
+        <v>1.9239999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -12031,10 +12408,10 @@
         <v>26</v>
       </c>
       <c r="F76" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G76">
-        <v>1.9239999999999999</v>
+        <v>1.9590000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -12048,16 +12425,16 @@
         <v>40</v>
       </c>
       <c r="D77" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
         <v>26</v>
       </c>
       <c r="F77" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G77">
-        <v>1.9590000000000001</v>
+        <v>2.4980000000000002</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -12077,10 +12454,10 @@
         <v>26</v>
       </c>
       <c r="F78" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G78">
-        <v>2.4980000000000002</v>
+        <v>2.5979999999999999</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -12100,10 +12477,10 @@
         <v>26</v>
       </c>
       <c r="F79" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G79">
-        <v>2.5979999999999999</v>
+        <v>2.665</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -12114,19 +12491,19 @@
         <v>36</v>
       </c>
       <c r="C80" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" t="s">
         <v>26</v>
       </c>
       <c r="F80" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G80">
-        <v>2.665</v>
+        <v>1.6859999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -12146,10 +12523,10 @@
         <v>26</v>
       </c>
       <c r="F81" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G81">
-        <v>1.6859999999999999</v>
+        <v>1.736</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -12169,10 +12546,10 @@
         <v>26</v>
       </c>
       <c r="F82" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G82">
-        <v>1.736</v>
+        <v>1.766</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -12186,16 +12563,16 @@
         <v>41</v>
       </c>
       <c r="D83" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" t="s">
         <v>26</v>
       </c>
       <c r="F83" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G83">
-        <v>1.766</v>
+        <v>2.2010000000000001</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -12215,10 +12592,10 @@
         <v>26</v>
       </c>
       <c r="F84" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G84">
-        <v>2.2010000000000001</v>
+        <v>2.2890000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -12238,38 +12615,38 @@
         <v>26</v>
       </c>
       <c r="F85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G85">
-        <v>2.2890000000000001</v>
+        <v>2.3479999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B86" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C86" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F86" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G86">
-        <v>2.3479999999999999</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B87" t="s">
         <v>39</v>
@@ -12287,12 +12664,12 @@
         <v>28</v>
       </c>
       <c r="G87">
-        <v>1.89</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B88" t="s">
         <v>39</v>
@@ -12310,12 +12687,12 @@
         <v>28</v>
       </c>
       <c r="G88">
-        <v>23.38</v>
+        <v>13.19</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B89" t="s">
         <v>39</v>
@@ -12333,12 +12710,12 @@
         <v>28</v>
       </c>
       <c r="G89">
-        <v>13.19</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B90" t="s">
         <v>39</v>
@@ -12353,15 +12730,15 @@
         <v>43</v>
       </c>
       <c r="F90" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G90">
-        <v>4.53</v>
+        <v>104.92</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B91" t="s">
         <v>39</v>
@@ -12379,12 +12756,12 @@
         <v>30</v>
       </c>
       <c r="G91">
-        <v>104.92</v>
+        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B92" t="s">
         <v>39</v>
@@ -12402,12 +12779,12 @@
         <v>30</v>
       </c>
       <c r="G92">
-        <v>66.400000000000006</v>
+        <v>79.209999999999994</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B93" t="s">
         <v>39</v>
@@ -12425,12 +12802,12 @@
         <v>30</v>
       </c>
       <c r="G93">
-        <v>79.209999999999994</v>
+        <v>56.32</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B94" t="s">
         <v>39</v>
@@ -12445,15 +12822,15 @@
         <v>43</v>
       </c>
       <c r="F94" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G94">
-        <v>56.32</v>
+        <v>3.7950000000000004</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B95" t="s">
         <v>39</v>
@@ -12471,12 +12848,12 @@
         <v>31</v>
       </c>
       <c r="G95">
-        <v>3.7950000000000004</v>
+        <v>4.7960000000000012</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B96" t="s">
         <v>39</v>
@@ -12494,12 +12871,12 @@
         <v>31</v>
       </c>
       <c r="G96">
-        <v>4.7960000000000012</v>
+        <v>4.6640000000000006</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B97" t="s">
         <v>39</v>
@@ -12517,12 +12894,12 @@
         <v>31</v>
       </c>
       <c r="G97">
-        <v>4.6640000000000006</v>
+        <v>4.6970000000000001</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B98" t="s">
         <v>39</v>
@@ -12531,21 +12908,21 @@
         <v>40</v>
       </c>
       <c r="D98" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" t="s">
         <v>43</v>
       </c>
       <c r="F98" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G98">
-        <v>4.6970000000000001</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B99" t="s">
         <v>39</v>
@@ -12563,12 +12940,12 @@
         <v>28</v>
       </c>
       <c r="G99">
-        <v>1.68</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B100" t="s">
         <v>39</v>
@@ -12586,12 +12963,12 @@
         <v>28</v>
       </c>
       <c r="G100">
-        <v>1.59</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B101" t="s">
         <v>39</v>
@@ -12609,12 +12986,12 @@
         <v>28</v>
       </c>
       <c r="G101">
-        <v>2.56</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B102" t="s">
         <v>39</v>
@@ -12629,15 +13006,15 @@
         <v>43</v>
       </c>
       <c r="F102" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G102">
-        <v>1.4</v>
+        <v>505.82</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B103" t="s">
         <v>39</v>
@@ -12655,12 +13032,12 @@
         <v>30</v>
       </c>
       <c r="G103">
-        <v>505.82</v>
+        <v>191.67</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B104" t="s">
         <v>39</v>
@@ -12678,12 +13055,12 @@
         <v>30</v>
       </c>
       <c r="G104">
-        <v>191.67</v>
+        <v>377.28</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B105" t="s">
         <v>39</v>
@@ -12701,12 +13078,12 @@
         <v>30</v>
       </c>
       <c r="G105">
-        <v>377.28</v>
+        <v>192.71</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B106" t="s">
         <v>39</v>
@@ -12721,15 +13098,15 @@
         <v>43</v>
       </c>
       <c r="F106" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G106">
-        <v>192.71</v>
+        <v>4.4660000000000002</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B107" t="s">
         <v>39</v>
@@ -12747,12 +13124,12 @@
         <v>31</v>
       </c>
       <c r="G107">
-        <v>4.4660000000000002</v>
+        <v>3.3880000000000003</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B108" t="s">
         <v>39</v>
@@ -12770,12 +13147,12 @@
         <v>31</v>
       </c>
       <c r="G108">
-        <v>3.3880000000000003</v>
+        <v>6.0500000000000007</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B109" t="s">
         <v>39</v>
@@ -12793,35 +13170,35 @@
         <v>31</v>
       </c>
       <c r="G109">
-        <v>6.0500000000000007</v>
+        <v>3.5420000000000007</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B110" t="s">
         <v>39</v>
       </c>
       <c r="C110" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D110" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110" t="s">
         <v>43</v>
       </c>
       <c r="F110" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G110">
-        <v>3.5420000000000007</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B111" t="s">
         <v>39</v>
@@ -12839,12 +13216,12 @@
         <v>28</v>
       </c>
       <c r="G111">
-        <v>1.89</v>
+        <v>23.38</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B112" t="s">
         <v>39</v>
@@ -12862,12 +13239,12 @@
         <v>28</v>
       </c>
       <c r="G112">
-        <v>23.38</v>
+        <v>13.19</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B113" t="s">
         <v>39</v>
@@ -12885,12 +13262,12 @@
         <v>28</v>
       </c>
       <c r="G113">
-        <v>13.19</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B114" t="s">
         <v>39</v>
@@ -12905,15 +13282,15 @@
         <v>43</v>
       </c>
       <c r="F114" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G114">
-        <v>4.53</v>
+        <v>104.92</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B115" t="s">
         <v>39</v>
@@ -12931,12 +13308,12 @@
         <v>30</v>
       </c>
       <c r="G115">
-        <v>104.92</v>
+        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B116" t="s">
         <v>39</v>
@@ -12954,12 +13331,12 @@
         <v>30</v>
       </c>
       <c r="G116">
-        <v>66.400000000000006</v>
+        <v>79.209999999999994</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B117" t="s">
         <v>39</v>
@@ -12977,12 +13354,12 @@
         <v>30</v>
       </c>
       <c r="G117">
-        <v>79.209999999999994</v>
+        <v>56.32</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B118" t="s">
         <v>39</v>
@@ -12997,15 +13374,15 @@
         <v>43</v>
       </c>
       <c r="F118" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G118">
-        <v>56.32</v>
+        <v>3.1050000000000004</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B119" t="s">
         <v>39</v>
@@ -13023,12 +13400,12 @@
         <v>31</v>
       </c>
       <c r="G119">
-        <v>3.1050000000000004</v>
+        <v>3.9240000000000004</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B120" t="s">
         <v>39</v>
@@ -13046,12 +13423,12 @@
         <v>31</v>
       </c>
       <c r="G120">
-        <v>3.9240000000000004</v>
+        <v>3.8160000000000003</v>
       </c>
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B121" t="s">
         <v>39</v>
@@ -13069,12 +13446,12 @@
         <v>31</v>
       </c>
       <c r="G121">
-        <v>3.8160000000000003</v>
+        <v>3.8429999999999995</v>
       </c>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B122" t="s">
         <v>39</v>
@@ -13083,21 +13460,21 @@
         <v>41</v>
       </c>
       <c r="D122" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E122" t="s">
         <v>43</v>
       </c>
       <c r="F122" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G122">
-        <v>3.8429999999999995</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B123" t="s">
         <v>39</v>
@@ -13115,12 +13492,12 @@
         <v>28</v>
       </c>
       <c r="G123">
-        <v>1.68</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B124" t="s">
         <v>39</v>
@@ -13138,12 +13515,12 @@
         <v>28</v>
       </c>
       <c r="G124">
-        <v>1.59</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B125" t="s">
         <v>39</v>
@@ -13161,12 +13538,12 @@
         <v>28</v>
       </c>
       <c r="G125">
-        <v>2.56</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B126" t="s">
         <v>39</v>
@@ -13181,15 +13558,15 @@
         <v>43</v>
       </c>
       <c r="F126" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G126">
-        <v>1.4</v>
+        <v>505.82</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B127" t="s">
         <v>39</v>
@@ -13207,12 +13584,12 @@
         <v>30</v>
       </c>
       <c r="G127">
-        <v>505.82</v>
+        <v>191.67</v>
       </c>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B128" t="s">
         <v>39</v>
@@ -13230,12 +13607,12 @@
         <v>30</v>
       </c>
       <c r="G128">
-        <v>191.67</v>
+        <v>377.28</v>
       </c>
     </row>
     <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B129" t="s">
         <v>39</v>
@@ -13253,12 +13630,12 @@
         <v>30</v>
       </c>
       <c r="G129">
-        <v>377.28</v>
+        <v>192.71</v>
       </c>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B130" t="s">
         <v>39</v>
@@ -13273,15 +13650,15 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G130">
-        <v>192.71</v>
+        <v>3.6539999999999999</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B131" t="s">
         <v>39</v>
@@ -13299,12 +13676,12 @@
         <v>31</v>
       </c>
       <c r="G131">
-        <v>3.6539999999999999</v>
+        <v>2.7720000000000002</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B132" t="s">
         <v>39</v>
@@ -13322,12 +13699,12 @@
         <v>31</v>
       </c>
       <c r="G132">
-        <v>2.7720000000000002</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B133" t="s">
         <v>39</v>
@@ -13345,30 +13722,30 @@
         <v>31</v>
       </c>
       <c r="G133">
-        <v>4.95</v>
+        <v>2.8980000000000001</v>
       </c>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B134" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C134" t="s">
         <v>41</v>
       </c>
       <c r="D134" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E134" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F134" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G134">
-        <v>2.8980000000000001</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -13388,10 +13765,10 @@
         <v>26</v>
       </c>
       <c r="F135" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G135">
-        <v>1.64</v>
+        <v>1.6879999999999999</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -13411,10 +13788,10 @@
         <v>26</v>
       </c>
       <c r="F136" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G136">
-        <v>1.6879999999999999</v>
+        <v>1.718</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -13428,16 +13805,16 @@
         <v>41</v>
       </c>
       <c r="D137" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E137" t="s">
         <v>26</v>
       </c>
       <c r="F137" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G137">
-        <v>1.718</v>
+        <v>2.1139999999999999</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -13457,10 +13834,10 @@
         <v>26</v>
       </c>
       <c r="F138" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G138">
-        <v>2.1139999999999999</v>
+        <v>2.1989999999999998</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -13480,10 +13857,10 @@
         <v>26</v>
       </c>
       <c r="F139" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G139">
-        <v>2.1989999999999998</v>
+        <v>2.2549999999999999</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -13494,19 +13871,19 @@
         <v>42</v>
       </c>
       <c r="C140" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D140" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E140" t="s">
         <v>26</v>
       </c>
       <c r="F140" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G140">
-        <v>2.2549999999999999</v>
+        <v>1.921</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -13526,10 +13903,10 @@
         <v>26</v>
       </c>
       <c r="F141" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G141">
-        <v>1.921</v>
+        <v>1.9770000000000001</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -13549,10 +13926,10 @@
         <v>26</v>
       </c>
       <c r="F142" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G142">
-        <v>1.9770000000000001</v>
+        <v>2.012</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -13566,16 +13943,16 @@
         <v>40</v>
       </c>
       <c r="D143" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E143" t="s">
         <v>26</v>
       </c>
       <c r="F143" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G143">
-        <v>2.012</v>
+        <v>2.5990000000000002</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -13595,10 +13972,10 @@
         <v>26</v>
       </c>
       <c r="F144" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G144">
-        <v>2.5990000000000002</v>
+        <v>2.7719999999999998</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -13618,32 +13995,9 @@
         <v>26</v>
       </c>
       <c r="F145" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G145">
-        <v>2.7719999999999998</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7">
-      <c r="A146" t="s">
-        <v>45</v>
-      </c>
-      <c r="B146" t="s">
-        <v>42</v>
-      </c>
-      <c r="C146" t="s">
-        <v>40</v>
-      </c>
-      <c r="D146" t="s">
-        <v>1</v>
-      </c>
-      <c r="E146" t="s">
-        <v>26</v>
-      </c>
-      <c r="F146" t="s">
-        <v>2</v>
-      </c>
-      <c r="G146">
         <v>2.7029999999999998</v>
       </c>
     </row>
@@ -13657,8 +14011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="I16:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>